<commit_message>
Feat: get data and proccess completed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auxis-my.sharepoint.com/personal/lmarquez_auxis_com/Documents/Documentos/UiPath/AUX-RPAChallenge_InvoiceExtraction/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B3608F-3036-452F-A3AE-C8A3F57474C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>RPAChallengeURL</t>
+  </si>
+  <si>
+    <t>https://www.rpachallenge.com/</t>
+  </si>
+  <si>
+    <t>TargetFolder</t>
+  </si>
+  <si>
+    <t>Data\Output\</t>
   </si>
 </sst>
 </file>
@@ -212,10 +224,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -238,10 +250,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,16 +553,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +620,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,8 +631,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,15 +1650,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,18 +1695,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1820,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2812,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>